<commit_message>
alterations to the install methods
</commit_message>
<xml_diff>
--- a/Junction_Capacity_Calculator.xlsx
+++ b/Junction_Capacity_Calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cswanston\Documents\GitHub\roundabout_capacity\dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aspence1\Documents\Scripts\roundabout_capacity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090237B2-9976-4E79-A2A9-803A0F6BEDE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E6FDBF-4179-4D32-936B-37B90F6BD947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18960" yWindow="4275" windowWidth="15120" windowHeight="8790" xr2:uid="{EED2B133-EB96-4C5B-AE9E-3165D2CA792E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EED2B133-EB96-4C5B-AE9E-3165D2CA792E}"/>
   </bookViews>
   <sheets>
     <sheet name="Control" sheetId="3" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>OD / ARMS</t>
   </si>
@@ -168,13 +168,7 @@
     <t>Output: Roundabout Flow Capacity</t>
   </si>
   <si>
-    <t>Error. Approach road half-width 1.0 falls below lower bound of 2.5</t>
-  </si>
-  <si>
     <t>No warnings advised</t>
-  </si>
-  <si>
-    <t>Error. Inscribed circle diameter 5.0 falls below lower bound of 28.0</t>
   </si>
 </sst>
 </file>
@@ -328,7 +322,7 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -672,17 +666,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10BBFF9D-FB56-402C-938D-B5CAA76C1F13}">
   <dimension ref="A2:AA28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.77734375" customWidth="1"/>
-    <col min="5" max="6" width="36.77734375" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="5" max="6" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" ht="25.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -713,12 +707,12 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -726,7 +720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -734,7 +728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -742,12 +736,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
@@ -755,10 +749,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -766,10 +760,10 @@
         <v>13</v>
       </c>
       <c r="C11" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -777,10 +771,10 @@
         <v>14</v>
       </c>
       <c r="C12" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -788,10 +782,10 @@
         <v>15</v>
       </c>
       <c r="C13" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -799,10 +793,10 @@
         <v>16</v>
       </c>
       <c r="C14" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>24</v>
       </c>
@@ -810,15 +804,15 @@
         <v>25</v>
       </c>
       <c r="C15" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>7</v>
       </c>
@@ -833,7 +827,7 @@
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
@@ -841,14 +835,14 @@
         <v>18</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
@@ -856,14 +850,14 @@
         <v>19</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
@@ -871,14 +865,14 @@
         <v>20</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
@@ -886,14 +880,14 @@
         <v>21</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>24</v>
       </c>
@@ -901,14 +895,14 @@
         <v>25</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
@@ -916,14 +910,14 @@
         <v>27</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>23</v>
       </c>
@@ -933,14 +927,14 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="9">
-        <v>2.3614043322627234</v>
+        <v>0.26382589253883831</v>
       </c>
     </row>
   </sheetData>
@@ -977,12 +971,12 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -999,91 +993,92 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" cm="1">
         <f t="array" aca="1" ref="B2:E5" ca="1">_xlfn.RANDARRAY(COUNT(B1:M1),COUNT(A2:A13),25,50,TRUE)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C2">
         <f ca="1"/>
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D2">
         <f ca="1"/>
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E2">
         <f ca="1"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3">
         <f ca="1"/>
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <f ca="1"/>
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3">
         <f ca="1"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <f ca="1"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4">
         <f ca="1"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <f ca="1"/>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <f ca="1"/>
+        <v>41</v>
+      </c>
+      <c r="E4">
+        <f ca="1"/>
         <v>48</v>
       </c>
-      <c r="E4">
-        <f ca="1"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5">
         <f ca="1"/>
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C5">
         <f ca="1"/>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5">
         <f ca="1"/>
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <f ca="1"/>
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>